<commit_message>
added new conductors and transformers to spreadsheets
</commit_message>
<xml_diff>
--- a/shift/catalogs/concentric_neutral_ug_cables.xlsx
+++ b/shift/catalogs/concentric_neutral_ug_cables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KDUWADI\Desktop\NREL_Projects\ciff_track_2\seeds_new\src\catalogs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epohl\Desktop\Tunisia\Current_SHIFT\shift\catalogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC75FE5-9D43-464C-A35A-322A13A8C073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFCB5C9-BBCC-4B3C-B6EA-00C8FE4B937E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-52995" yWindow="5115" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="46">
   <si>
     <t>name</t>
   </si>
@@ -146,13 +146,37 @@
   </si>
   <si>
     <t>runit</t>
+  </si>
+  <si>
+    <t>cross_section</t>
+  </si>
+  <si>
+    <t>cross_section_units</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Almelec_50</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>ALMELEC</t>
+  </si>
+  <si>
+    <t>Almelec_120</t>
+  </si>
+  <si>
+    <t>Almelec_240</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +190,19 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -207,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -215,6 +252,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -282,9 +323,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3020AEE8-08E0-4FF5-813B-0772BDF47E6F}" name="Table1" displayName="Table1" ref="A1:R15" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
-  <autoFilter ref="A1:R15" xr:uid="{3020AEE8-08E0-4FF5-813B-0772BDF47E6F}"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3020AEE8-08E0-4FF5-813B-0772BDF47E6F}" name="Table1" displayName="Table1" ref="A1:T18" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+  <autoFilter ref="A1:T18" xr:uid="{3020AEE8-08E0-4FF5-813B-0772BDF47E6F}"/>
+  <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{7D252BF8-5391-437B-BBF2-4A67D723026A}" name="name"/>
     <tableColumn id="2" xr3:uid="{B858BBFD-51B5-4EFA-B07A-4E55D71B522A}" name="diastrand"/>
     <tableColumn id="3" xr3:uid="{98BBDB8E-7B61-42E5-AE56-CED5B370F8A0}" name="inslayer"/>
@@ -303,6 +344,8 @@
     <tableColumn id="16" xr3:uid="{548C41C4-6D6E-4099-ABD0-66DC8BBDE9F6}" name="kV"/>
     <tableColumn id="17" xr3:uid="{E270552E-9336-4288-88AA-0D3E87C29EE5}" name="neutral_type"/>
     <tableColumn id="18" xr3:uid="{659A106C-B865-4278-9186-17A32FA131FA}" name="material"/>
+    <tableColumn id="19" xr3:uid="{A4D24B13-A99E-4B16-B4CA-8575E4728F92}" name="cross_section"/>
+    <tableColumn id="20" xr3:uid="{CB286FF0-509D-4F84-A48E-3283D1B07B97}" name="cross_section_units"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -593,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,7 +663,7 @@
     <col min="18" max="18" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -675,8 +718,14 @@
       <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="S1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -731,8 +780,14 @@
       <c r="R2" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="S2" s="3">
+        <v>0</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -787,8 +842,14 @@
       <c r="R3" t="s">
         <v>18</v>
       </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -843,8 +904,14 @@
       <c r="R4" t="s">
         <v>18</v>
       </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -899,8 +966,14 @@
       <c r="R5" t="s">
         <v>18</v>
       </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -955,8 +1028,14 @@
       <c r="R6" t="s">
         <v>18</v>
       </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1011,8 +1090,14 @@
       <c r="R7" t="s">
         <v>18</v>
       </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1067,8 +1152,14 @@
       <c r="R8" t="s">
         <v>18</v>
       </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1123,8 +1214,14 @@
       <c r="R9" t="s">
         <v>18</v>
       </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1179,8 +1276,14 @@
       <c r="R10" t="s">
         <v>18</v>
       </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1235,8 +1338,14 @@
       <c r="R11" t="s">
         <v>18</v>
       </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1291,8 +1400,14 @@
       <c r="R12" t="s">
         <v>18</v>
       </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -1347,8 +1462,14 @@
       <c r="R13" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="S13" s="3">
+        <v>0</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1403,8 +1524,14 @@
       <c r="R14" t="s">
         <v>18</v>
       </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1459,10 +1586,198 @@
       <c r="R15" t="s">
         <v>18</v>
       </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="F16" s="1"/>
-      <c r="L16" s="1"/>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="6">
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="C16">
+        <v>0.315</v>
+      </c>
+      <c r="D16">
+        <v>0.31</v>
+      </c>
+      <c r="E16">
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="1">
+        <v>16</v>
+      </c>
+      <c r="G16">
+        <v>0.94</v>
+      </c>
+      <c r="H16">
+        <v>4.8675000000000003E-2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="6">
+        <v>14.872199999999999</v>
+      </c>
+      <c r="K16">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="L16" s="1">
+        <v>205</v>
+      </c>
+      <c r="M16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16">
+        <v>2.0799999999999998E-3</v>
+      </c>
+      <c r="O16" t="s">
+        <v>16</v>
+      </c>
+      <c r="P16">
+        <v>30</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>17</v>
+      </c>
+      <c r="R16" t="s">
+        <v>43</v>
+      </c>
+      <c r="S16">
+        <v>50</v>
+      </c>
+      <c r="T16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="6">
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="C17">
+        <v>0.315</v>
+      </c>
+      <c r="D17">
+        <v>0.49</v>
+      </c>
+      <c r="E17">
+        <v>1.69</v>
+      </c>
+      <c r="F17" s="1">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H17">
+        <v>5.4840500000000007E-2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="6">
+        <v>14.872199999999999</v>
+      </c>
+      <c r="K17">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="L17" s="1">
+        <v>295</v>
+      </c>
+      <c r="M17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N17">
+        <v>2.0799999999999998E-3</v>
+      </c>
+      <c r="O17" t="s">
+        <v>16</v>
+      </c>
+      <c r="P17">
+        <v>30</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>17</v>
+      </c>
+      <c r="R17" t="s">
+        <v>43</v>
+      </c>
+      <c r="S17">
+        <v>120</v>
+      </c>
+      <c r="T17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="6">
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="C18">
+        <v>0.315</v>
+      </c>
+      <c r="D18">
+        <v>0.69</v>
+      </c>
+      <c r="E18">
+        <v>1.89</v>
+      </c>
+      <c r="F18" s="1">
+        <v>25</v>
+      </c>
+      <c r="G18">
+        <v>1.3199999999999998</v>
+      </c>
+      <c r="H18">
+        <v>6.1330500000000003E-2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="6">
+        <v>14.872199999999999</v>
+      </c>
+      <c r="K18">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="L18" s="1">
+        <v>390</v>
+      </c>
+      <c r="M18" t="s">
+        <v>42</v>
+      </c>
+      <c r="N18">
+        <v>2.0799999999999998E-3</v>
+      </c>
+      <c r="O18" t="s">
+        <v>16</v>
+      </c>
+      <c r="P18">
+        <v>30</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>17</v>
+      </c>
+      <c r="R18" t="s">
+        <v>43</v>
+      </c>
+      <c r="S18">
+        <v>240</v>
+      </c>
+      <c r="T18" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
reverted catalogs back to original
</commit_message>
<xml_diff>
--- a/shift/catalogs/concentric_neutral_ug_cables.xlsx
+++ b/shift/catalogs/concentric_neutral_ug_cables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epohl\Desktop\Tunisia\Current_SHIFT\shift\catalogs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KDUWADI\Desktop\NREL_Projects\ciff_track_2\seeds_new\src\catalogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFCB5C9-BBCC-4B3C-B6EA-00C8FE4B937E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC75FE5-9D43-464C-A35A-322A13A8C073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-52995" yWindow="5115" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="38">
   <si>
     <t>name</t>
   </si>
@@ -146,37 +146,13 @@
   </si>
   <si>
     <t>runit</t>
-  </si>
-  <si>
-    <t>cross_section</t>
-  </si>
-  <si>
-    <t>cross_section_units</t>
-  </si>
-  <si>
-    <t>mm</t>
-  </si>
-  <si>
-    <t>Almelec_50</t>
-  </si>
-  <si>
-    <t>km</t>
-  </si>
-  <si>
-    <t>ALMELEC</t>
-  </si>
-  <si>
-    <t>Almelec_120</t>
-  </si>
-  <si>
-    <t>Almelec_240</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,19 +166,6 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -244,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -252,10 +215,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -323,9 +282,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3020AEE8-08E0-4FF5-813B-0772BDF47E6F}" name="Table1" displayName="Table1" ref="A1:T18" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
-  <autoFilter ref="A1:T18" xr:uid="{3020AEE8-08E0-4FF5-813B-0772BDF47E6F}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3020AEE8-08E0-4FF5-813B-0772BDF47E6F}" name="Table1" displayName="Table1" ref="A1:R15" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+  <autoFilter ref="A1:R15" xr:uid="{3020AEE8-08E0-4FF5-813B-0772BDF47E6F}"/>
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{7D252BF8-5391-437B-BBF2-4A67D723026A}" name="name"/>
     <tableColumn id="2" xr3:uid="{B858BBFD-51B5-4EFA-B07A-4E55D71B522A}" name="diastrand"/>
     <tableColumn id="3" xr3:uid="{98BBDB8E-7B61-42E5-AE56-CED5B370F8A0}" name="inslayer"/>
@@ -344,8 +303,6 @@
     <tableColumn id="16" xr3:uid="{548C41C4-6D6E-4099-ABD0-66DC8BBDE9F6}" name="kV"/>
     <tableColumn id="17" xr3:uid="{E270552E-9336-4288-88AA-0D3E87C29EE5}" name="neutral_type"/>
     <tableColumn id="18" xr3:uid="{659A106C-B865-4278-9186-17A32FA131FA}" name="material"/>
-    <tableColumn id="19" xr3:uid="{A4D24B13-A99E-4B16-B4CA-8575E4728F92}" name="cross_section"/>
-    <tableColumn id="20" xr3:uid="{CB286FF0-509D-4F84-A48E-3283D1B07B97}" name="cross_section_units"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -636,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -663,7 +620,7 @@
     <col min="18" max="18" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -718,14 +675,8 @@
       <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -780,14 +731,8 @@
       <c r="R2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="3">
-        <v>0</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -842,14 +787,8 @@
       <c r="R3" t="s">
         <v>18</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -904,14 +843,8 @@
       <c r="R4" t="s">
         <v>18</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -966,14 +899,8 @@
       <c r="R5" t="s">
         <v>18</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1028,14 +955,8 @@
       <c r="R6" t="s">
         <v>18</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1090,14 +1011,8 @@
       <c r="R7" t="s">
         <v>18</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1152,14 +1067,8 @@
       <c r="R8" t="s">
         <v>18</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1214,14 +1123,8 @@
       <c r="R9" t="s">
         <v>18</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1276,14 +1179,8 @@
       <c r="R10" t="s">
         <v>18</v>
       </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1338,14 +1235,8 @@
       <c r="R11" t="s">
         <v>18</v>
       </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1400,14 +1291,8 @@
       <c r="R12" t="s">
         <v>18</v>
       </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -1462,14 +1347,8 @@
       <c r="R13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S13" s="3">
-        <v>0</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1524,14 +1403,8 @@
       <c r="R14" t="s">
         <v>18</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1586,198 +1459,10 @@
       <c r="R15" t="s">
         <v>18</v>
       </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="6">
-        <v>6.4100000000000004E-2</v>
-      </c>
-      <c r="C16">
-        <v>0.315</v>
-      </c>
-      <c r="D16">
-        <v>0.31</v>
-      </c>
-      <c r="E16">
-        <v>1.5</v>
-      </c>
-      <c r="F16" s="1">
-        <v>16</v>
-      </c>
-      <c r="G16">
-        <v>0.94</v>
-      </c>
-      <c r="H16">
-        <v>4.8675000000000003E-2</v>
-      </c>
-      <c r="I16" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="6">
-        <v>14.872199999999999</v>
-      </c>
-      <c r="K16">
-        <v>0.82399999999999995</v>
-      </c>
-      <c r="L16" s="1">
-        <v>205</v>
-      </c>
-      <c r="M16" t="s">
-        <v>42</v>
-      </c>
-      <c r="N16">
-        <v>2.0799999999999998E-3</v>
-      </c>
-      <c r="O16" t="s">
-        <v>16</v>
-      </c>
-      <c r="P16">
-        <v>30</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>17</v>
-      </c>
-      <c r="R16" t="s">
-        <v>43</v>
-      </c>
-      <c r="S16">
-        <v>50</v>
-      </c>
-      <c r="T16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="6">
-        <v>6.4100000000000004E-2</v>
-      </c>
-      <c r="C17">
-        <v>0.315</v>
-      </c>
-      <c r="D17">
-        <v>0.49</v>
-      </c>
-      <c r="E17">
-        <v>1.69</v>
-      </c>
-      <c r="F17" s="1">
-        <v>16</v>
-      </c>
-      <c r="G17">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="H17">
-        <v>5.4840500000000007E-2</v>
-      </c>
-      <c r="I17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="6">
-        <v>14.872199999999999</v>
-      </c>
-      <c r="K17">
-        <v>0.32700000000000001</v>
-      </c>
-      <c r="L17" s="1">
-        <v>295</v>
-      </c>
-      <c r="M17" t="s">
-        <v>42</v>
-      </c>
-      <c r="N17">
-        <v>2.0799999999999998E-3</v>
-      </c>
-      <c r="O17" t="s">
-        <v>16</v>
-      </c>
-      <c r="P17">
-        <v>30</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>17</v>
-      </c>
-      <c r="R17" t="s">
-        <v>43</v>
-      </c>
-      <c r="S17">
-        <v>120</v>
-      </c>
-      <c r="T17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="6">
-        <v>6.4100000000000004E-2</v>
-      </c>
-      <c r="C18">
-        <v>0.315</v>
-      </c>
-      <c r="D18">
-        <v>0.69</v>
-      </c>
-      <c r="E18">
-        <v>1.89</v>
-      </c>
-      <c r="F18" s="1">
-        <v>25</v>
-      </c>
-      <c r="G18">
-        <v>1.3199999999999998</v>
-      </c>
-      <c r="H18">
-        <v>6.1330500000000003E-2</v>
-      </c>
-      <c r="I18" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" s="6">
-        <v>14.872199999999999</v>
-      </c>
-      <c r="K18">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="L18" s="1">
-        <v>390</v>
-      </c>
-      <c r="M18" t="s">
-        <v>42</v>
-      </c>
-      <c r="N18">
-        <v>2.0799999999999998E-3</v>
-      </c>
-      <c r="O18" t="s">
-        <v>16</v>
-      </c>
-      <c r="P18">
-        <v>30</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>17</v>
-      </c>
-      <c r="R18" t="s">
-        <v>43</v>
-      </c>
-      <c r="S18">
-        <v>240</v>
-      </c>
-      <c r="T18" t="s">
-        <v>40</v>
-      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="F16" s="1"/>
+      <c r="L16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>